<commit_message>
thong nhat buoi hop + logo ispace
</commit_message>
<xml_diff>
--- a/Design/Nội dung công việc.xlsx
+++ b/Design/Nội dung công việc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>DANH SÁCH CÔNG VIỆC</t>
   </si>
@@ -95,13 +95,22 @@
   </si>
   <si>
     <t>Dự kiến 1-&gt;2M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doi voi POA thi tren tung don  vừa có phần tải về để người dùng sửa và up lên </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chị tuyến gửi lại </t>
+  </si>
+  <si>
+    <t>Chị tuyến gưi lại các trường dữ liệu kế thừa mầu xanh,  các trường dữ liệu mầu đỏ sẽ được nhập mới</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +122,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -249,19 +265,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,7 +586,7 @@
   <dimension ref="B3:V36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +638,7 @@
       <c r="V4" s="7"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -650,7 +667,7 @@
       <c r="V5" s="7"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="8" t="s">
@@ -675,7 +692,7 @@
       <c r="V6" s="7"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="8" t="s">
@@ -700,7 +717,7 @@
       <c r="V7" s="7"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="8" t="s">
@@ -725,7 +742,7 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8" t="s">
@@ -750,7 +767,7 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -811,7 +828,9 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="K12" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -861,7 +880,9 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -884,7 +905,9 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -923,7 +946,7 @@
       <c r="V16" s="7"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="5"/>
@@ -950,7 +973,7 @@
       <c r="V17" s="7"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
@@ -975,7 +998,7 @@
       <c r="V18" s="7"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
@@ -1000,7 +1023,7 @@
       <c r="V19" s="7"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1025,7 +1048,7 @@
       <c r="V20" s="7"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
         <v>1</v>
@@ -1050,7 +1073,7 @@
       <c r="V21" s="7"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1073,7 +1096,7 @@
       <c r="V22" s="7"/>
     </row>
     <row r="23" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6" t="s">
         <v>2</v>
@@ -1098,7 +1121,7 @@
       <c r="V23" s="7"/>
     </row>
     <row r="24" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1121,7 +1144,7 @@
       <c r="V24" s="7"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6" t="s">
         <v>3</v>
@@ -1146,7 +1169,7 @@
       <c r="V25" s="7"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1169,7 +1192,7 @@
       <c r="V26" s="7"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6" t="s">
         <v>4</v>
@@ -1355,7 +1378,7 @@
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E35" s="6"/>

</xml_diff>